<commit_message>
docs: sync updates - 2026-02-12 04:30
</commit_message>
<xml_diff>
--- a/semiconductor_roadmaps/china/Huawei_Roadmap.xlsx
+++ b/semiconductor_roadmaps/china/Huawei_Roadmap.xlsx
@@ -542,227 +542,196 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>发布时间</t>
+          <t>2024-Q1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>产品</t>
+          <t>2024-Q4</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>制程</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>AI性能</t>
+          <t>2026</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>主要特性</t>
+          <t>2027</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>备注</t>
+          <t>2028</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-Q1</t>
+          <t>Ascend 910B</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ascend 910B</t>
+          <t>Ascend 910C</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7nm (国内)</t>
+          <t>Ascend 950</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>FP16 400 TFLOPS</t>
+          <t>Ascend 960</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>当前主力</t>
+          <t>Ascend 970</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>已发布</t>
+          <t>下一代</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-Q4</t>
+          <t>7nm (国内)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ascend 910C</t>
+          <t>7nm (国内)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7nm (国内)</t>
+          <t>5nm (国内)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>FP16 ~500 TFLOPS</t>
+          <t>5nm (国内)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>性能提升</t>
+          <t>3nm (国内)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>已发布</t>
+          <t>2nm (国内)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-Q3</t>
+          <t>FP16 400 TFLOPS</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ascend 920 (Cannondale)</t>
+          <t>FP16 ~500 TFLOPS</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5nm (国内)</t>
+          <t>FP16 ~1 PFLOPS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FP16 ~800 TFLOPS</t>
+          <t>FP16 ~2 PFLOPS</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>新一代</t>
+          <t>FP16 ~4 PFLOPS</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025发布</t>
+          <t>FP4 ~8 ZettaFLOPS</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-Q1</t>
+          <t>当前主力</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ascend 950系列</t>
+          <t>性能提升</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5nm (国内)</t>
+          <t>新一代</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FP16 ~1.5 PFLOPS</t>
+          <t>下一代</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>高性能</t>
+          <t>下一代</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2026发布</t>
+          <t>远期目标</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2027-Q1</t>
+          <t>已发布</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ascend 960系列</t>
+          <t>已发布</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3nm (国内)</t>
+          <t>2026发布</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>FP16 ~3 PFLOPS</t>
+          <t>2027目标</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>下一代</t>
+          <t>2028目标</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2027发布</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2028-Q1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Ascend 下一代</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2nm (国内)</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>FP4 4 ZettaFLOPS</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>远期目标</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
           <t>2028目标</t>
         </is>
       </c>
     </row>
+    <row r="9"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>